<commit_message>
montant à payer en lettre et en chiffre
</commit_message>
<xml_diff>
--- a/modele_facture.xlsx
+++ b/modele_facture.xlsx
@@ -591,7 +591,7 @@
       </c>
       <c r="E2" s="5" t="inlineStr">
         <is>
-          <t>JB</t>
+          <t>zer</t>
         </is>
       </c>
       <c r="G2" s="6" t="inlineStr"/>
@@ -822,17 +822,17 @@
     <row r="18">
       <c r="A18" s="21" t="inlineStr">
         <is>
-          <t>258</t>
+          <t>40</t>
         </is>
       </c>
       <c r="B18" s="21" t="inlineStr">
         <is>
-          <t>lait concentré</t>
+          <t>lait en poudre</t>
         </is>
       </c>
       <c r="C18" s="21" t="inlineStr"/>
       <c r="D18" s="21" t="n">
-        <v>34000</v>
+        <v>20000</v>
       </c>
       <c r="E18" s="21" t="n">
         <v>24000</v>
@@ -841,66 +841,26 @@
         <v>0</v>
       </c>
       <c r="G18" s="21" t="n">
-        <v>58000</v>
+        <v>44000</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="21" t="inlineStr">
-        <is>
-          <t>256</t>
-        </is>
-      </c>
-      <c r="B19" s="21" t="inlineStr">
-        <is>
-          <t>lait en poudre</t>
-        </is>
-      </c>
-      <c r="C19" s="21" t="inlineStr">
-        <is>
-          <t>310/1</t>
-        </is>
-      </c>
-      <c r="D19" s="21" t="n">
-        <v>20000</v>
-      </c>
-      <c r="E19" s="21" t="n">
-        <v>24000</v>
-      </c>
-      <c r="F19" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G19" s="21" t="n">
-        <v>44000</v>
-      </c>
+      <c r="A19" s="25" t="n"/>
+      <c r="B19" s="25" t="n"/>
+      <c r="C19" s="25" t="n"/>
+      <c r="D19" s="25" t="n"/>
+      <c r="E19" s="25" t="n"/>
+      <c r="F19" s="25" t="n"/>
+      <c r="G19" s="25" t="n"/>
     </row>
     <row r="20">
-      <c r="A20" s="21" t="inlineStr">
-        <is>
-          <t>257</t>
-        </is>
-      </c>
-      <c r="B20" s="21" t="inlineStr">
-        <is>
-          <t>yaourt</t>
-        </is>
-      </c>
-      <c r="C20" s="21" t="inlineStr">
-        <is>
-          <t>310/2</t>
-        </is>
-      </c>
-      <c r="D20" s="21" t="n">
-        <v>19000</v>
-      </c>
-      <c r="E20" s="21" t="n">
-        <v>24000</v>
-      </c>
-      <c r="F20" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="G20" s="21" t="n">
-        <v>43000</v>
-      </c>
+      <c r="A20" s="25" t="n"/>
+      <c r="B20" s="25" t="n"/>
+      <c r="C20" s="25" t="n"/>
+      <c r="D20" s="25" t="n"/>
+      <c r="E20" s="25" t="n"/>
+      <c r="F20" s="25" t="n"/>
+      <c r="G20" s="25" t="n"/>
     </row>
     <row r="21">
       <c r="A21" s="25" t="n"/>

</xml_diff>

<commit_message>
ajout de separateur de millier au champ avec montant
</commit_message>
<xml_diff>
--- a/modele_facture.xlsx
+++ b/modele_facture.xlsx
@@ -822,7 +822,7 @@
     <row r="18">
       <c r="A18" s="21" t="inlineStr">
         <is>
-          <t>40</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B18" s="21" t="inlineStr">
@@ -832,7 +832,7 @@
       </c>
       <c r="C18" s="21" t="inlineStr"/>
       <c r="D18" s="21" t="n">
-        <v>20000</v>
+        <v>180000</v>
       </c>
       <c r="E18" s="21" t="n">
         <v>24000</v>
@@ -841,7 +841,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="21" t="n">
-        <v>44000</v>
+        <v>204000</v>
       </c>
     </row>
     <row r="19">

</xml_diff>

<commit_message>
recherche facture à partir du numéro de facture
</commit_message>
<xml_diff>
--- a/modele_facture.xlsx
+++ b/modele_facture.xlsx
@@ -591,7 +591,7 @@
       </c>
       <c r="E2" s="5" t="inlineStr">
         <is>
-          <t>zer</t>
+          <t>JB</t>
         </is>
       </c>
       <c r="G2" s="6" t="inlineStr"/>
@@ -822,7 +822,7 @@
     <row r="18">
       <c r="A18" s="21" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>10</t>
         </is>
       </c>
       <c r="B18" s="21" t="inlineStr">

</xml_diff>

<commit_message>
radio bouton facture normale et facture proforma
</commit_message>
<xml_diff>
--- a/modele_facture.xlsx
+++ b/modele_facture.xlsx
@@ -591,7 +591,7 @@
       </c>
       <c r="E2" s="5" t="inlineStr">
         <is>
-          <t>JB</t>
+          <t>Socobis</t>
         </is>
       </c>
       <c r="G2" s="6" t="inlineStr"/>
@@ -822,26 +822,26 @@
     <row r="18">
       <c r="A18" s="21" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>20</t>
         </is>
       </c>
       <c r="B18" s="21" t="inlineStr">
         <is>
-          <t>lait en poudre</t>
+          <t>Frego</t>
         </is>
       </c>
       <c r="C18" s="21" t="inlineStr"/>
       <c r="D18" s="21" t="n">
-        <v>180000</v>
+        <v>150000</v>
       </c>
       <c r="E18" s="21" t="n">
-        <v>24000</v>
+        <v>240000</v>
       </c>
       <c r="F18" s="21" t="n">
         <v>0</v>
       </c>
       <c r="G18" s="21" t="n">
-        <v>204000</v>
+        <v>390000</v>
       </c>
     </row>
     <row r="19">

</xml_diff>

<commit_message>
modification et suppression d'un produit analysé
</commit_message>
<xml_diff>
--- a/modele_facture.xlsx
+++ b/modele_facture.xlsx
@@ -591,7 +591,7 @@
       </c>
       <c r="E2" s="5" t="inlineStr">
         <is>
-          <t>Socobis</t>
+          <t>jB</t>
         </is>
       </c>
       <c r="G2" s="6" t="inlineStr"/>
@@ -822,17 +822,17 @@
     <row r="18">
       <c r="A18" s="21" t="inlineStr">
         <is>
-          <t>20</t>
+          <t>1</t>
         </is>
       </c>
       <c r="B18" s="21" t="inlineStr">
         <is>
-          <t>Frego</t>
+          <t>Fanta</t>
         </is>
       </c>
       <c r="C18" s="21" t="inlineStr"/>
       <c r="D18" s="21" t="n">
-        <v>150000</v>
+        <v>180000</v>
       </c>
       <c r="E18" s="21" t="n">
         <v>240000</v>
@@ -841,7 +841,7 @@
         <v>0</v>
       </c>
       <c r="G18" s="21" t="n">
-        <v>390000</v>
+        <v>420000</v>
       </c>
     </row>
     <row r="19">

</xml_diff>